<commit_message>
Se adicionan casos pruebas de invalidos.
</commit_message>
<xml_diff>
--- a/docs/CasosPruebas.xlsx
+++ b/docs/CasosPruebas.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris_martinez\Desktop\Meli\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803F8004-4CF2-4340-9D22-2B0A1955B5F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D1A5AF99-38B8-4FBC-8671-6BADD133C738}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="4X4" sheetId="1" r:id="rId1"/>
     <sheet name="10X10" sheetId="2" r:id="rId2"/>
+    <sheet name="Invalidas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="7">
   <si>
     <t>A</t>
   </si>
@@ -45,11 +40,14 @@
   <si>
     <t>Test Case</t>
   </si>
+  <si>
+    <t>B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,7 +91,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -313,11 +311,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -342,27 +384,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -375,12 +399,88 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -681,77 +781,77 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E6D8BF-3139-4F3E-ACC9-88B3FE678FD6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50:T50"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="W51" sqref="W51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="8.77734375" style="6"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="2.08984375" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="6"/>
+    <col min="4" max="4" width="1.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="2.109375" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="6"/>
     <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="2.08984375" customWidth="1"/>
-    <col min="16" max="16" width="8.7265625" style="6"/>
+    <col min="11" max="11" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2.109375" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" style="6"/>
     <col min="17" max="17" width="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="21"/>
-      <c r="P2" s="37" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
+      <c r="P2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="Q2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="21"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B3" s="26">
-        <v>1</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="38"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
@@ -764,10 +864,10 @@
         <v>3</v>
       </c>
       <c r="H3" s="7"/>
-      <c r="I3" s="26">
+      <c r="I3" s="33">
         <v>5</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="12" t="s">
@@ -781,10 +881,10 @@
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="26">
+      <c r="P3" s="33">
         <v>7</v>
       </c>
-      <c r="Q3" s="23" t="s">
+      <c r="Q3" s="20" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="12" t="s">
@@ -793,13 +893,13 @@
       <c r="S3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="35" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B4" s="27"/>
-      <c r="C4" s="24" t="s">
+      <c r="T3" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="34"/>
+      <c r="C4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -812,8 +912,8 @@
         <v>2</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="29" t="s">
+      <c r="I4" s="34"/>
+      <c r="J4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -827,8 +927,8 @@
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="24" t="s">
+      <c r="P4" s="34"/>
+      <c r="Q4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -841,9 +941,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B5" s="27"/>
-      <c r="C5" s="24" t="s">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B5" s="34"/>
+      <c r="C5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -856,8 +956,8 @@
         <v>3</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="29" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="23" t="s">
         <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -871,8 +971,8 @@
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="24" t="s">
+      <c r="P5" s="34"/>
+      <c r="Q5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -885,9 +985,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="28"/>
-      <c r="C6" s="25" t="s">
+    <row r="6" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="35"/>
+      <c r="C6" s="22" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -900,8 +1000,8 @@
         <v>2</v>
       </c>
       <c r="H6" s="7"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="30" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="K6" s="9" t="s">
@@ -915,8 +1015,8 @@
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="25" t="s">
+      <c r="P6" s="35"/>
+      <c r="Q6" s="22" t="s">
         <v>0</v>
       </c>
       <c r="R6" s="9" t="s">
@@ -946,39 +1046,39 @@
       <c r="P7"/>
     </row>
     <row r="8" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="I8" s="37" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="I8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="21"/>
-      <c r="P8" s="37" t="s">
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="38"/>
+      <c r="P8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q8" s="22" t="s">
+      <c r="Q8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="21"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B9" s="26">
-        <v>2</v>
-      </c>
-      <c r="C9" s="23" t="s">
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="38"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="33">
+        <v>2</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -992,10 +1092,10 @@
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="26">
+      <c r="I9" s="33">
         <v>6</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="26" t="s">
         <v>0</v>
       </c>
       <c r="K9" s="12" t="s">
@@ -1009,10 +1109,10 @@
       </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
-      <c r="P9" s="26">
+      <c r="P9" s="33">
         <v>8</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="Q9" s="20" t="s">
         <v>0</v>
       </c>
       <c r="R9" s="18" t="s">
@@ -1021,13 +1121,13 @@
       <c r="S9" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="T9" s="35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B10" s="27"/>
-      <c r="C10" s="33" t="s">
+      <c r="T9" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="34"/>
+      <c r="C10" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1041,8 +1141,8 @@
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="33" t="s">
+      <c r="I10" s="34"/>
+      <c r="J10" s="27" t="s">
         <v>2</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1056,8 +1156,8 @@
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="29" t="s">
+      <c r="P10" s="34"/>
+      <c r="Q10" s="23" t="s">
         <v>0</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -1070,9 +1170,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B11" s="27"/>
-      <c r="C11" s="33" t="s">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="34"/>
+      <c r="C11" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1086,8 +1186,8 @@
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="33" t="s">
+      <c r="I11" s="34"/>
+      <c r="J11" s="27" t="s">
         <v>2</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -1101,8 +1201,8 @@
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="29" t="s">
+      <c r="P11" s="34"/>
+      <c r="Q11" s="23" t="s">
         <v>0</v>
       </c>
       <c r="R11" s="1" t="s">
@@ -1115,9 +1215,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="28"/>
-      <c r="C12" s="34" t="s">
+    <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="35"/>
+      <c r="C12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -1131,8 +1231,8 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="34" t="s">
+      <c r="I12" s="35"/>
+      <c r="J12" s="28" t="s">
         <v>2</v>
       </c>
       <c r="K12" s="9" t="s">
@@ -1146,8 +1246,8 @@
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="25" t="s">
+      <c r="P12" s="35"/>
+      <c r="Q12" s="22" t="s">
         <v>0</v>
       </c>
       <c r="R12" s="8" t="s">
@@ -1176,32 +1276,32 @@
       <c r="P13"/>
     </row>
     <row r="14" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="P14" s="37" t="s">
+      <c r="P14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q14" s="22" t="s">
+      <c r="Q14" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="21"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B15" s="26">
-        <v>3</v>
-      </c>
-      <c r="C15" s="32" t="s">
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="38"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B15" s="33">
+        <v>3</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -1210,15 +1310,15 @@
       <c r="E15" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="29" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="P15" s="26">
+      <c r="P15" s="33">
         <v>9</v>
       </c>
-      <c r="Q15" s="23" t="s">
+      <c r="Q15" s="20" t="s">
         <v>0</v>
       </c>
       <c r="R15" s="12" t="s">
@@ -1227,13 +1327,13 @@
       <c r="S15" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T15" s="35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B16" s="27"/>
-      <c r="C16" s="33" t="s">
+      <c r="T15" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B16" s="34"/>
+      <c r="C16" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1247,8 +1347,8 @@
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="33" t="s">
+      <c r="P16" s="34"/>
+      <c r="Q16" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R16" s="2" t="s">
@@ -1261,9 +1361,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B17" s="27"/>
-      <c r="C17" s="33" t="s">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B17" s="34"/>
+      <c r="C17" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1277,8 +1377,8 @@
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="33" t="s">
+      <c r="P17" s="34"/>
+      <c r="Q17" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R17" s="2" t="s">
@@ -1291,9 +1391,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="28"/>
-      <c r="C18" s="25" t="s">
+    <row r="18" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="35"/>
+      <c r="C18" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -1307,8 +1407,8 @@
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="25" t="s">
+      <c r="P18" s="35"/>
+      <c r="Q18" s="22" t="s">
         <v>0</v>
       </c>
       <c r="R18" s="9" t="s">
@@ -1331,32 +1431,32 @@
       <c r="P19"/>
     </row>
     <row r="20" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-      <c r="P20" s="37" t="s">
+      <c r="P20" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q20" s="22" t="s">
+      <c r="Q20" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="21"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B21" s="26">
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="38"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B21" s="33">
         <v>4</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="26" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="12" t="s">
@@ -1365,15 +1465,15 @@
       <c r="E21" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="29" t="s">
         <v>0</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="P21" s="26">
+      <c r="P21" s="33">
         <v>10</v>
       </c>
-      <c r="Q21" s="23" t="s">
+      <c r="Q21" s="20" t="s">
         <v>0</v>
       </c>
       <c r="R21" s="18" t="s">
@@ -1382,13 +1482,13 @@
       <c r="S21" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="T21" s="35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B22" s="27"/>
-      <c r="C22" s="33" t="s">
+      <c r="T21" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B22" s="34"/>
+      <c r="C22" s="27" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1402,8 +1502,8 @@
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="24" t="s">
+      <c r="P22" s="34"/>
+      <c r="Q22" s="21" t="s">
         <v>0</v>
       </c>
       <c r="R22" s="1" t="s">
@@ -1416,9 +1516,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B23" s="27"/>
-      <c r="C23" s="33" t="s">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B23" s="34"/>
+      <c r="C23" s="27" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1432,8 +1532,8 @@
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="24" t="s">
+      <c r="P23" s="34"/>
+      <c r="Q23" s="21" t="s">
         <v>0</v>
       </c>
       <c r="R23" s="1" t="s">
@@ -1446,9 +1546,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="28"/>
-      <c r="C24" s="34" t="s">
+    <row r="24" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="35"/>
+      <c r="C24" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -1462,8 +1562,8 @@
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="25" t="s">
+      <c r="P24" s="35"/>
+      <c r="Q24" s="22" t="s">
         <v>0</v>
       </c>
       <c r="R24" s="9" t="s">
@@ -1490,21 +1590,21 @@
     <row r="26" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="P26" s="37" t="s">
+      <c r="P26" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q26" s="22" t="s">
+      <c r="Q26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="21"/>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="P27" s="26">
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="38"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P27" s="33">
         <v>11</v>
       </c>
-      <c r="Q27" s="23" t="s">
+      <c r="Q27" s="20" t="s">
         <v>0</v>
       </c>
       <c r="R27" s="18" t="s">
@@ -1513,13 +1613,13 @@
       <c r="S27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="T27" s="35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="P28" s="27"/>
-      <c r="Q28" s="33" t="s">
+      <c r="T27" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P28" s="34"/>
+      <c r="Q28" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R28" s="1" t="s">
@@ -1532,9 +1632,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="P29" s="27"/>
-      <c r="Q29" s="33" t="s">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P29" s="34"/>
+      <c r="Q29" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R29" s="1" t="s">
@@ -1547,9 +1647,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P30" s="28"/>
-      <c r="Q30" s="34" t="s">
+    <row r="30" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P30" s="35"/>
+      <c r="Q30" s="28" t="s">
         <v>2</v>
       </c>
       <c r="R30" s="9" t="s">
@@ -1566,21 +1666,21 @@
       <c r="P31"/>
     </row>
     <row r="32" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P32" s="37" t="s">
+      <c r="P32" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q32" s="22" t="s">
+      <c r="Q32" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="21"/>
-    </row>
-    <row r="33" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P33" s="26">
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="38"/>
+    </row>
+    <row r="33" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P33" s="33">
         <v>12</v>
       </c>
-      <c r="Q33" s="32" t="s">
+      <c r="Q33" s="26" t="s">
         <v>0</v>
       </c>
       <c r="R33" s="12" t="s">
@@ -1589,13 +1689,13 @@
       <c r="S33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T33" s="35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P34" s="27"/>
-      <c r="Q34" s="33" t="s">
+      <c r="T33" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P34" s="34"/>
+      <c r="Q34" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R34" s="1" t="s">
@@ -1608,9 +1708,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P35" s="27"/>
-      <c r="Q35" s="33" t="s">
+    <row r="35" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P35" s="34"/>
+      <c r="Q35" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R35" s="1" t="s">
@@ -1623,9 +1723,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P36" s="28"/>
-      <c r="Q36" s="25" t="s">
+    <row r="36" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P36" s="35"/>
+      <c r="Q36" s="22" t="s">
         <v>0</v>
       </c>
       <c r="R36" s="8" t="s">
@@ -1638,25 +1738,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P37"/>
     </row>
-    <row r="38" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P38" s="37" t="s">
+    <row r="38" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P38" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q38" s="22" t="s">
+      <c r="Q38" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="21"/>
-    </row>
-    <row r="39" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P39" s="26">
+      <c r="R38" s="37"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="38"/>
+    </row>
+    <row r="39" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P39" s="33">
         <v>13</v>
       </c>
-      <c r="Q39" s="23" t="s">
+      <c r="Q39" s="20" t="s">
         <v>1</v>
       </c>
       <c r="R39" s="12" t="s">
@@ -1669,9 +1769,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P40" s="27"/>
-      <c r="Q40" s="24" t="s">
+    <row r="40" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P40" s="34"/>
+      <c r="Q40" s="21" t="s">
         <v>1</v>
       </c>
       <c r="R40" s="1" t="s">
@@ -1684,9 +1784,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P41" s="27"/>
-      <c r="Q41" s="24" t="s">
+    <row r="41" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P41" s="34"/>
+      <c r="Q41" s="21" t="s">
         <v>1</v>
       </c>
       <c r="R41" s="1" t="s">
@@ -1699,9 +1799,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P42" s="28"/>
-      <c r="Q42" s="25" t="s">
+    <row r="42" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P42" s="35"/>
+      <c r="Q42" s="22" t="s">
         <v>1</v>
       </c>
       <c r="R42" s="8" t="s">
@@ -1714,25 +1814,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P43"/>
     </row>
-    <row r="44" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P44" s="37" t="s">
+    <row r="44" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P44" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q44" s="22" t="s">
+      <c r="Q44" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R44" s="20"/>
-      <c r="S44" s="20"/>
-      <c r="T44" s="21"/>
-    </row>
-    <row r="45" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P45" s="26">
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="38"/>
+    </row>
+    <row r="45" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P45" s="33">
         <v>14</v>
       </c>
-      <c r="Q45" s="32" t="s">
+      <c r="Q45" s="26" t="s">
         <v>0</v>
       </c>
       <c r="R45" s="18" t="s">
@@ -1745,9 +1845,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P46" s="27"/>
-      <c r="Q46" s="33" t="s">
+    <row r="46" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P46" s="34"/>
+      <c r="Q46" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R46" s="2" t="s">
@@ -1760,9 +1860,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P47" s="27"/>
-      <c r="Q47" s="33" t="s">
+    <row r="47" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P47" s="34"/>
+      <c r="Q47" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R47" s="2" t="s">
@@ -1775,9 +1875,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P48" s="28"/>
-      <c r="Q48" s="25" t="s">
+    <row r="48" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P48" s="35"/>
+      <c r="Q48" s="22" t="s">
         <v>1</v>
       </c>
       <c r="R48" s="8" t="s">
@@ -1790,23 +1890,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="50" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P50" s="37" t="s">
+    <row r="49" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P50" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q50" s="22" t="s">
+      <c r="Q50" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="R50" s="20"/>
-      <c r="S50" s="20"/>
-      <c r="T50" s="21"/>
-    </row>
-    <row r="51" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P51" s="26">
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="38"/>
+    </row>
+    <row r="51" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P51" s="33">
         <v>15</v>
       </c>
-      <c r="Q51" s="23" t="s">
+      <c r="Q51" s="20" t="s">
         <v>1</v>
       </c>
       <c r="R51" s="12" t="s">
@@ -1815,13 +1915,13 @@
       <c r="S51" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T51" s="35" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P52" s="27"/>
-      <c r="Q52" s="24" t="s">
+      <c r="T51" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P52" s="34"/>
+      <c r="Q52" s="21" t="s">
         <v>1</v>
       </c>
       <c r="R52" s="1" t="s">
@@ -1834,9 +1934,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="16:20" x14ac:dyDescent="0.35">
-      <c r="P53" s="27"/>
-      <c r="Q53" s="24" t="s">
+    <row r="53" spans="16:20" x14ac:dyDescent="0.3">
+      <c r="P53" s="34"/>
+      <c r="Q53" s="21" t="s">
         <v>1</v>
       </c>
       <c r="R53" s="2" t="s">
@@ -1849,9 +1949,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P54" s="28"/>
-      <c r="Q54" s="25" t="s">
+    <row r="54" spans="16:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P54" s="35"/>
+      <c r="Q54" s="22" t="s">
         <v>1</v>
       </c>
       <c r="R54" s="8" t="s">
@@ -1866,13 +1966,19 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="P51:P54"/>
-    <mergeCell ref="P3:P6"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="P15:P18"/>
-    <mergeCell ref="P21:P24"/>
-    <mergeCell ref="P27:P30"/>
-    <mergeCell ref="P33:P36"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="Q14:T14"/>
+    <mergeCell ref="Q20:T20"/>
+    <mergeCell ref="Q26:T26"/>
     <mergeCell ref="Q38:T38"/>
     <mergeCell ref="Q44:T44"/>
     <mergeCell ref="Q50:T50"/>
@@ -1882,20 +1988,14 @@
     <mergeCell ref="I9:I12"/>
     <mergeCell ref="P39:P42"/>
     <mergeCell ref="P45:P48"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="Q14:T14"/>
-    <mergeCell ref="Q20:T20"/>
-    <mergeCell ref="Q26:T26"/>
     <mergeCell ref="Q32:T32"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="P51:P54"/>
+    <mergeCell ref="P3:P6"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="P15:P18"/>
+    <mergeCell ref="P21:P24"/>
+    <mergeCell ref="P27:P30"/>
+    <mergeCell ref="P33:P36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1903,72 +2003,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49298EF-EEEE-4CAB-8627-A8FE15EDF24D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="2" max="2" width="8.77734375" style="6"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="6"/>
-    <col min="15" max="16" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" style="6"/>
+    <col min="15" max="16" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="2.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
-      <c r="N2" s="37" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="N2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="21"/>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B3" s="26">
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="38"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B3" s="33">
         <v>16</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
@@ -1980,7 +2080,7 @@
       <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="30" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="12" t="s">
@@ -1998,10 +2098,10 @@
       <c r="L3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="26">
+      <c r="N3" s="33">
         <v>19</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="P3" s="1" t="s">
@@ -2032,9 +2132,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B4" s="27"/>
-      <c r="C4" s="24" t="s">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B4" s="34"/>
+      <c r="C4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2064,8 +2164,8 @@
       <c r="L4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="27"/>
-      <c r="O4" s="24" t="s">
+      <c r="N4" s="34"/>
+      <c r="O4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="P4" s="1" t="s">
@@ -2096,9 +2196,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B5" s="27"/>
-      <c r="C5" s="24" t="s">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B5" s="34"/>
+      <c r="C5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2128,8 +2228,8 @@
       <c r="L5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="24" t="s">
+      <c r="N5" s="34"/>
+      <c r="O5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -2160,9 +2260,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B6" s="27"/>
-      <c r="C6" s="24" t="s">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B6" s="34"/>
+      <c r="C6" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2192,8 +2292,8 @@
       <c r="L6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="27"/>
-      <c r="O6" s="24" t="s">
+      <c r="N6" s="34"/>
+      <c r="O6" s="21" t="s">
         <v>0</v>
       </c>
       <c r="P6" s="1" t="s">
@@ -2224,9 +2324,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B7" s="27"/>
-      <c r="C7" s="29" t="s">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B7" s="34"/>
+      <c r="C7" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2256,8 +2356,8 @@
       <c r="L7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="27"/>
-      <c r="O7" s="38" t="s">
+      <c r="N7" s="34"/>
+      <c r="O7" s="32" t="s">
         <v>0</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -2288,9 +2388,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B8" s="27"/>
-      <c r="C8" s="29" t="s">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B8" s="34"/>
+      <c r="C8" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2320,8 +2420,8 @@
       <c r="L8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="27"/>
-      <c r="O8" s="38" t="s">
+      <c r="N8" s="34"/>
+      <c r="O8" s="32" t="s">
         <v>0</v>
       </c>
       <c r="P8" s="1" t="s">
@@ -2352,9 +2452,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B9" s="27"/>
-      <c r="C9" s="29" t="s">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B9" s="34"/>
+      <c r="C9" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2384,8 +2484,8 @@
       <c r="L9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N9" s="27"/>
-      <c r="O9" s="38" t="s">
+      <c r="N9" s="34"/>
+      <c r="O9" s="32" t="s">
         <v>0</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -2416,9 +2516,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B10" s="27"/>
-      <c r="C10" s="29" t="s">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B10" s="34"/>
+      <c r="C10" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2448,8 +2548,8 @@
       <c r="L10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="27"/>
-      <c r="O10" s="38" t="s">
+      <c r="N10" s="34"/>
+      <c r="O10" s="32" t="s">
         <v>0</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -2480,9 +2580,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B11" s="27"/>
-      <c r="C11" s="29" t="s">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B11" s="34"/>
+      <c r="C11" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2512,8 +2612,8 @@
       <c r="L11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="27"/>
-      <c r="O11" s="29" t="s">
+      <c r="N11" s="34"/>
+      <c r="O11" s="23" t="s">
         <v>2</v>
       </c>
       <c r="P11" s="1" t="s">
@@ -2544,9 +2644,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="28"/>
-      <c r="C12" s="30" t="s">
+    <row r="12" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="35"/>
+      <c r="C12" s="24" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -2576,8 +2676,8 @@
       <c r="L12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="28"/>
-      <c r="O12" s="30" t="s">
+      <c r="N12" s="35"/>
+      <c r="O12" s="24" t="s">
         <v>3</v>
       </c>
       <c r="P12" s="9" t="s">
@@ -2610,39 +2710,39 @@
     </row>
     <row r="13" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="21"/>
-      <c r="N14" s="37" t="s">
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="38"/>
+      <c r="N14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="O14" s="22" t="s">
+      <c r="O14" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="20"/>
-      <c r="X14" s="21"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B15" s="26">
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="38"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B15" s="33">
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -2675,7 +2775,7 @@
       <c r="L15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="26">
+      <c r="N15" s="33">
         <v>20</v>
       </c>
       <c r="O15" s="2" t="s">
@@ -2709,8 +2809,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B16" s="27"/>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B16" s="34"/>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
@@ -2741,7 +2841,7 @@
       <c r="L16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N16" s="27"/>
+      <c r="N16" s="34"/>
       <c r="O16" s="2" t="s">
         <v>0</v>
       </c>
@@ -2773,8 +2873,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B17" s="27"/>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B17" s="34"/>
       <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2805,7 +2905,7 @@
       <c r="L17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N17" s="27"/>
+      <c r="N17" s="34"/>
       <c r="O17" s="2" t="s">
         <v>0</v>
       </c>
@@ -2837,8 +2937,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B18" s="27"/>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B18" s="34"/>
       <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2869,7 +2969,7 @@
       <c r="L18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N18" s="27"/>
+      <c r="N18" s="34"/>
       <c r="O18" s="2" t="s">
         <v>0</v>
       </c>
@@ -2901,8 +3001,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B19" s="27"/>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B19" s="34"/>
       <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +3033,7 @@
       <c r="L19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N19" s="27"/>
+      <c r="N19" s="34"/>
       <c r="O19" s="4" t="s">
         <v>0</v>
       </c>
@@ -2965,8 +3065,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B20" s="27"/>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B20" s="34"/>
       <c r="C20" s="3" t="s">
         <v>0</v>
       </c>
@@ -2997,7 +3097,7 @@
       <c r="L20" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N20" s="27"/>
+      <c r="N20" s="34"/>
       <c r="O20" s="4" t="s">
         <v>0</v>
       </c>
@@ -3029,8 +3129,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B21" s="27"/>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B21" s="34"/>
       <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
@@ -3061,7 +3161,7 @@
       <c r="L21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N21" s="27"/>
+      <c r="N21" s="34"/>
       <c r="O21" s="4" t="s">
         <v>0</v>
       </c>
@@ -3093,8 +3193,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B22" s="27"/>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B22" s="34"/>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
@@ -3125,7 +3225,7 @@
       <c r="L22" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N22" s="27"/>
+      <c r="N22" s="34"/>
       <c r="O22" s="4" t="s">
         <v>0</v>
       </c>
@@ -3157,8 +3257,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B23" s="27"/>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B23" s="34"/>
       <c r="C23" s="3" t="s">
         <v>2</v>
       </c>
@@ -3189,7 +3289,7 @@
       <c r="L23" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N23" s="27"/>
+      <c r="N23" s="34"/>
       <c r="O23" s="3" t="s">
         <v>2</v>
       </c>
@@ -3221,8 +3321,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="28"/>
+    <row r="24" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="35"/>
       <c r="C24" s="17" t="s">
         <v>3</v>
       </c>
@@ -3253,7 +3353,7 @@
       <c r="L24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="N24" s="28"/>
+      <c r="N24" s="35"/>
       <c r="O24" s="17" t="s">
         <v>3</v>
       </c>
@@ -3287,39 +3387,39 @@
     </row>
     <row r="25" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="26" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="21"/>
-      <c r="N26" s="37" t="s">
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="38"/>
+      <c r="N26" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="O26" s="22" t="s">
+      <c r="O26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="20"/>
-      <c r="X26" s="21"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B27" s="26">
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="38"/>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B27" s="33">
         <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -3352,7 +3452,7 @@
       <c r="L27" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="26">
+      <c r="N27" s="33">
         <v>21</v>
       </c>
       <c r="O27" s="2" t="s">
@@ -3386,8 +3486,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B28" s="27"/>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B28" s="34"/>
       <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
@@ -3418,7 +3518,7 @@
       <c r="L28" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N28" s="27"/>
+      <c r="N28" s="34"/>
       <c r="O28" s="5" t="s">
         <v>1</v>
       </c>
@@ -3450,8 +3550,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B29" s="27"/>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B29" s="34"/>
       <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
@@ -3482,7 +3582,7 @@
       <c r="L29" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N29" s="27"/>
+      <c r="N29" s="34"/>
       <c r="O29" s="5" t="s">
         <v>3</v>
       </c>
@@ -3514,8 +3614,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B30" s="27"/>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B30" s="34"/>
       <c r="C30" s="3" t="s">
         <v>2</v>
       </c>
@@ -3546,7 +3646,7 @@
       <c r="L30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N30" s="27"/>
+      <c r="N30" s="34"/>
       <c r="O30" s="5" t="s">
         <v>1</v>
       </c>
@@ -3578,8 +3678,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B31" s="27"/>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B31" s="34"/>
       <c r="C31" s="3" t="s">
         <v>0</v>
       </c>
@@ -3610,7 +3710,7 @@
       <c r="L31" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N31" s="27"/>
+      <c r="N31" s="34"/>
       <c r="O31" s="2" t="s">
         <v>2</v>
       </c>
@@ -3642,8 +3742,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B32" s="27"/>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B32" s="34"/>
       <c r="C32" s="3" t="s">
         <v>0</v>
       </c>
@@ -3674,7 +3774,7 @@
       <c r="L32" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N32" s="27"/>
+      <c r="N32" s="34"/>
       <c r="O32" s="3" t="s">
         <v>0</v>
       </c>
@@ -3706,8 +3806,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B33" s="27"/>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B33" s="34"/>
       <c r="C33" s="3" t="s">
         <v>0</v>
       </c>
@@ -3738,7 +3838,7 @@
       <c r="L33" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N33" s="27"/>
+      <c r="N33" s="34"/>
       <c r="O33" s="3" t="s">
         <v>0</v>
       </c>
@@ -3770,8 +3870,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B34" s="27"/>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B34" s="34"/>
       <c r="C34" s="3" t="s">
         <v>1</v>
       </c>
@@ -3802,7 +3902,7 @@
       <c r="L34" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N34" s="27"/>
+      <c r="N34" s="34"/>
       <c r="O34" s="3" t="s">
         <v>1</v>
       </c>
@@ -3834,8 +3934,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B35" s="27"/>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B35" s="34"/>
       <c r="C35" s="3" t="s">
         <v>2</v>
       </c>
@@ -3866,7 +3966,7 @@
       <c r="L35" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="N35" s="27"/>
+      <c r="N35" s="34"/>
       <c r="O35" s="3" t="s">
         <v>2</v>
       </c>
@@ -3898,8 +3998,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="28"/>
+    <row r="36" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="35"/>
       <c r="C36" s="17" t="s">
         <v>3</v>
       </c>
@@ -3930,7 +4030,7 @@
       <c r="L36" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="N36" s="28"/>
+      <c r="N36" s="35"/>
       <c r="O36" s="17" t="s">
         <v>3</v>
       </c>
@@ -3964,6 +4064,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="O2:X2"/>
+    <mergeCell ref="N3:N12"/>
+    <mergeCell ref="B15:B24"/>
     <mergeCell ref="B27:B36"/>
     <mergeCell ref="N27:N36"/>
     <mergeCell ref="N15:N24"/>
@@ -3971,11 +4076,297 @@
     <mergeCell ref="O14:X14"/>
     <mergeCell ref="O26:X26"/>
     <mergeCell ref="C26:L26"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="O2:X2"/>
-    <mergeCell ref="N3:N12"/>
-    <mergeCell ref="B15:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" customWidth="1"/>
+    <col min="4" max="4" width="6.21875" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="H3" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="33">
+        <v>22</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="42">
+        <v>25</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="34"/>
+      <c r="C5" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="43"/>
+      <c r="I5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="34"/>
+      <c r="C6" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="43"/>
+      <c r="I6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="35"/>
+      <c r="C7" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="44"/>
+      <c r="I7" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="33">
+        <v>23</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="34"/>
+      <c r="C12" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="35"/>
+      <c r="C13" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="33">
+        <v>24</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="34"/>
+      <c r="C18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="34"/>
+      <c r="C19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="35"/>
+      <c r="C20" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se implementa logica de analisis del dna
</commit_message>
<xml_diff>
--- a/docs/CasosPruebas.xlsx
+++ b/docs/CasosPruebas.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Borrador\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E5B3B4-578D-474C-97C1-1531F98DC2C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="4X4" sheetId="1" r:id="rId1"/>
     <sheet name="10X10" sheetId="2" r:id="rId2"/>
     <sheet name="Invalidas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,14 +411,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -435,14 +429,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,14 +447,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,7 +485,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -796,75 +790,74 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="AE32" sqref="AE32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="8.85546875" style="6"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" customWidth="1"/>
-    <col min="8" max="8" width="2.08984375" customWidth="1"/>
-    <col min="9" max="9" width="8.81640625" style="6"/>
+    <col min="4" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="6"/>
     <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" customWidth="1"/>
-    <col min="15" max="15" width="2.08984375" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" style="6"/>
+    <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="6"/>
     <col min="17" max="17" width="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
       <c r="H2" s="7"/>
       <c r="I2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="45"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
       <c r="P2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="43" t="s">
+      <c r="Q2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="45"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="51"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="46">
         <v>1</v>
       </c>
@@ -925,7 +918,7 @@
         <v>"AACT"</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="47"/>
       <c r="C4" s="21" t="s">
         <v>0</v>
@@ -980,7 +973,7 @@
         <v>"AGTT"</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
       <c r="C5" s="21" t="s">
         <v>0</v>
@@ -1035,7 +1028,7 @@
         <v>"ATCT"</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="48"/>
       <c r="C6" s="22" t="s">
         <v>0</v>
@@ -1090,7 +1083,7 @@
         <v>"AGTT"</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>G3&amp;","&amp;G4&amp;","&amp;G5&amp;","&amp;G6</f>
         <v>"ATCG","AGTC","ATCG","AGTC"</v>
@@ -1121,7 +1114,7 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1137,36 +1130,36 @@
       <c r="O8" s="7"/>
       <c r="P8"/>
     </row>
-    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="45"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="51"/>
       <c r="I9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="45"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
       <c r="P9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="43" t="s">
+      <c r="Q9" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="45"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="R9" s="50"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="51"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="46">
         <v>2</v>
       </c>
@@ -1227,7 +1220,7 @@
         <v>"AAAA"</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
       <c r="C11" s="27" t="s">
         <v>2</v>
@@ -1266,7 +1259,7 @@
       <c r="O11" s="7"/>
       <c r="P11" s="47"/>
       <c r="Q11" s="23" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>3</v>
@@ -1279,10 +1272,10 @@
       </c>
       <c r="U11" t="str">
         <f t="shared" ref="U11:U13" si="5">CHAR(34)&amp;Q11&amp;R11&amp;S11&amp;T11&amp;CHAR(34)</f>
-        <v>"AGTC"</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+        <v>"GGTC"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
       <c r="C12" s="27" t="s">
         <v>2</v>
@@ -1337,7 +1330,7 @@
         <v>"ATCG"</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="48"/>
       <c r="C13" s="28" t="s">
         <v>2</v>
@@ -1392,7 +1385,7 @@
         <v>"AAAA"</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>G10&amp;","&amp;G11&amp;","&amp;G12&amp;","&amp;G13</f>
         <v>"ATCG","CACG","CTAG","CTCA"</v>
@@ -1415,7 +1408,7 @@
       <c r="N14" s="7"/>
       <c r="O14" t="str">
         <f>U10&amp;","&amp;U11&amp;","&amp;U12&amp;","&amp;U13</f>
-        <v>"AAAA","AGTC","ATCG","AAAA"</v>
+        <v>"AAAA","GGTC","ATCG","AAAA"</v>
       </c>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
@@ -1424,7 +1417,7 @@
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1439,29 +1432,29 @@
       <c r="O15" s="7"/>
       <c r="P15"/>
     </row>
-    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="51"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="P16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q16" s="43" t="s">
+      <c r="Q16" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44"/>
-      <c r="T16" s="45"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="R16" s="50"/>
+      <c r="S16" s="50"/>
+      <c r="T16" s="51"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B17" s="46">
         <v>3</v>
       </c>
@@ -1502,7 +1495,7 @@
         <v>"ATCA"</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B18" s="47"/>
       <c r="C18" s="27" t="s">
         <v>2</v>
@@ -1539,7 +1532,7 @@
         <v>"CAAG"</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" s="47"/>
       <c r="C19" s="27" t="s">
         <v>2</v>
@@ -1576,7 +1569,7 @@
         <v>"CAAG"</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="48"/>
       <c r="C20" s="22" t="s">
         <v>1</v>
@@ -1613,7 +1606,7 @@
         <v>"ATCA"</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>G17&amp;","&amp;G18&amp;","&amp;G19&amp;","&amp;G20</f>
         <v>"TTCT","CGTG","CTGG","TTCC"</v>
@@ -1642,7 +1635,7 @@
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1651,29 +1644,29 @@
       <c r="H22" s="7"/>
       <c r="P22"/>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="45"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="51"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="P23" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q23" s="43" t="s">
+      <c r="Q23" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R23" s="44"/>
-      <c r="S23" s="44"/>
-      <c r="T23" s="45"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="51"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="46">
         <v>4</v>
       </c>
@@ -1714,7 +1707,7 @@
         <v>"AAAA"</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="47"/>
       <c r="C25" s="27" t="s">
         <v>3</v>
@@ -1751,7 +1744,7 @@
         <v>"AACG"</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B26" s="47"/>
       <c r="C26" s="27" t="s">
         <v>1</v>
@@ -1788,7 +1781,7 @@
         <v>"ATAG"</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="48"/>
       <c r="C27" s="28" t="s">
         <v>3</v>
@@ -1825,7 +1818,7 @@
         <v>"ATCC"</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>G24&amp;","&amp;G25&amp;","&amp;G26&amp;","&amp;G27</f>
         <v>"TTCA","GGTA","TTCA","GGTA"</v>
@@ -1854,7 +1847,7 @@
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -1865,20 +1858,20 @@
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
     </row>
-    <row r="30" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="P30" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q30" s="43" t="s">
+      <c r="Q30" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R30" s="44"/>
-      <c r="S30" s="44"/>
-      <c r="T30" s="45"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="51"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="P31" s="46">
         <v>11</v>
       </c>
@@ -1899,13 +1892,13 @@
         <v>"AAAA"</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="P32" s="47"/>
       <c r="Q32" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>2</v>
@@ -1915,10 +1908,10 @@
       </c>
       <c r="U32" t="str">
         <f t="shared" ref="U32:U34" si="10">CHAR(34)&amp;Q32&amp;R32&amp;S32&amp;T32&amp;CHAR(34)</f>
-        <v>"CACA"</v>
-      </c>
-    </row>
-    <row r="33" spans="15:21" x14ac:dyDescent="0.35">
+        <v>"CTCA"</v>
+      </c>
+    </row>
+    <row r="33" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P33" s="47"/>
       <c r="Q33" s="27" t="s">
         <v>2</v>
@@ -1937,7 +1930,7 @@
         <v>"CTAA"</v>
       </c>
     </row>
-    <row r="34" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P34" s="48"/>
       <c r="Q34" s="28" t="s">
         <v>2</v>
@@ -1956,28 +1949,28 @@
         <v>"CTCA"</v>
       </c>
     </row>
-    <row r="35" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="35" spans="15:21" x14ac:dyDescent="0.25">
       <c r="O35" t="str">
         <f>U31&amp;","&amp;U32&amp;","&amp;U33&amp;","&amp;U34</f>
-        <v>"AAAA","CACA","CTAA","CTCA"</v>
+        <v>"AAAA","CTCA","CTAA","CTCA"</v>
       </c>
       <c r="P35"/>
     </row>
-    <row r="36" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P36"/>
     </row>
-    <row r="37" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P37" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q37" s="43" t="s">
+      <c r="Q37" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R37" s="44"/>
-      <c r="S37" s="44"/>
-      <c r="T37" s="45"/>
-    </row>
-    <row r="38" spans="15:21" x14ac:dyDescent="0.35">
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
+      <c r="T37" s="51"/>
+    </row>
+    <row r="38" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P38" s="46">
         <v>12</v>
       </c>
@@ -1998,13 +1991,13 @@
         <v>"ATCA"</v>
       </c>
     </row>
-    <row r="39" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P39" s="47"/>
       <c r="Q39" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S39" s="1" t="s">
         <v>2</v>
@@ -2014,10 +2007,10 @@
       </c>
       <c r="U39" t="str">
         <f t="shared" ref="U39:U41" si="11">CHAR(34)&amp;Q39&amp;R39&amp;S39&amp;T39&amp;CHAR(34)</f>
-        <v>"CACA"</v>
-      </c>
-    </row>
-    <row r="40" spans="15:21" x14ac:dyDescent="0.35">
+        <v>"CTCA"</v>
+      </c>
+    </row>
+    <row r="40" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P40" s="47"/>
       <c r="Q40" s="27" t="s">
         <v>2</v>
@@ -2036,7 +2029,7 @@
         <v>"CTAA"</v>
       </c>
     </row>
-    <row r="41" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P41" s="48"/>
       <c r="Q41" s="22" t="s">
         <v>0</v>
@@ -2055,28 +2048,28 @@
         <v>"AAAA"</v>
       </c>
     </row>
-    <row r="42" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="15:21" x14ac:dyDescent="0.25">
       <c r="O42" t="str">
         <f>U38&amp;","&amp;U39&amp;","&amp;U40&amp;","&amp;U41</f>
-        <v>"ATCA","CACA","CTAA","AAAA"</v>
+        <v>"ATCA","CTCA","CTAA","AAAA"</v>
       </c>
       <c r="P42"/>
     </row>
-    <row r="43" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P43"/>
     </row>
-    <row r="44" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P44" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q44" s="43" t="s">
+      <c r="Q44" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R44" s="44"/>
-      <c r="S44" s="44"/>
-      <c r="T44" s="45"/>
-    </row>
-    <row r="45" spans="15:21" x14ac:dyDescent="0.35">
+      <c r="R44" s="50"/>
+      <c r="S44" s="50"/>
+      <c r="T44" s="51"/>
+    </row>
+    <row r="45" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P45" s="46">
         <v>13</v>
       </c>
@@ -2097,7 +2090,7 @@
         <v>"TTCG"</v>
       </c>
     </row>
-    <row r="46" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P46" s="47"/>
       <c r="Q46" s="21" t="s">
         <v>1</v>
@@ -2116,7 +2109,7 @@
         <v>"TACG"</v>
       </c>
     </row>
-    <row r="47" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="47" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P47" s="47"/>
       <c r="Q47" s="21" t="s">
         <v>1</v>
@@ -2135,7 +2128,7 @@
         <v>"TTAG"</v>
       </c>
     </row>
-    <row r="48" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P48" s="48"/>
       <c r="Q48" s="22" t="s">
         <v>1</v>
@@ -2154,28 +2147,28 @@
         <v>"TTTT"</v>
       </c>
     </row>
-    <row r="49" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="49" spans="15:21" x14ac:dyDescent="0.25">
       <c r="O49" t="str">
         <f>U45&amp;","&amp;U46&amp;","&amp;U47&amp;","&amp;U48</f>
         <v>"TTCG","TACG","TTAG","TTTT"</v>
       </c>
       <c r="P49"/>
     </row>
-    <row r="50" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P50"/>
     </row>
-    <row r="51" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P51" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q51" s="43" t="s">
+      <c r="Q51" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R51" s="44"/>
-      <c r="S51" s="44"/>
-      <c r="T51" s="45"/>
-    </row>
-    <row r="52" spans="15:21" x14ac:dyDescent="0.35">
+      <c r="R51" s="50"/>
+      <c r="S51" s="50"/>
+      <c r="T51" s="51"/>
+    </row>
+    <row r="52" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P52" s="46">
         <v>14</v>
       </c>
@@ -2196,7 +2189,7 @@
         <v>"ATCG"</v>
       </c>
     </row>
-    <row r="53" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="53" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P53" s="47"/>
       <c r="Q53" s="27" t="s">
         <v>2</v>
@@ -2215,7 +2208,7 @@
         <v>"CTCG"</v>
       </c>
     </row>
-    <row r="54" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="54" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P54" s="47"/>
       <c r="Q54" s="27" t="s">
         <v>2</v>
@@ -2234,7 +2227,7 @@
         <v>"CTAG"</v>
       </c>
     </row>
-    <row r="55" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P55" s="48"/>
       <c r="Q55" s="22" t="s">
         <v>1</v>
@@ -2253,26 +2246,26 @@
         <v>"TTTT"</v>
       </c>
     </row>
-    <row r="56" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="56" spans="15:21" x14ac:dyDescent="0.25">
       <c r="O56" t="str">
         <f>U52&amp;","&amp;U53&amp;","&amp;U54&amp;","&amp;U55</f>
         <v>"ATCG","CTCG","CTAG","TTTT"</v>
       </c>
       <c r="P56"/>
     </row>
-    <row r="57" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="58" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P58" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Q58" s="43" t="s">
+      <c r="Q58" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R58" s="44"/>
-      <c r="S58" s="44"/>
-      <c r="T58" s="45"/>
-    </row>
-    <row r="59" spans="15:21" x14ac:dyDescent="0.35">
+      <c r="R58" s="50"/>
+      <c r="S58" s="50"/>
+      <c r="T58" s="51"/>
+    </row>
+    <row r="59" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P59" s="46">
         <v>15</v>
       </c>
@@ -2293,7 +2286,7 @@
         <v>"TTCT"</v>
       </c>
     </row>
-    <row r="60" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="60" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P60" s="47"/>
       <c r="Q60" s="21" t="s">
         <v>1</v>
@@ -2312,7 +2305,7 @@
         <v>"TATG"</v>
       </c>
     </row>
-    <row r="61" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="61" spans="15:21" x14ac:dyDescent="0.25">
       <c r="P61" s="47"/>
       <c r="Q61" s="21" t="s">
         <v>1</v>
@@ -2331,7 +2324,7 @@
         <v>"TTAG"</v>
       </c>
     </row>
-    <row r="62" spans="15:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="15:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P62" s="48"/>
       <c r="Q62" s="22" t="s">
         <v>1</v>
@@ -2350,7 +2343,7 @@
         <v>"TTTT"</v>
       </c>
     </row>
-    <row r="63" spans="15:21" x14ac:dyDescent="0.35">
+    <row r="63" spans="15:21" x14ac:dyDescent="0.25">
       <c r="O63" t="str">
         <f>U59&amp;","&amp;U60&amp;","&amp;U61&amp;","&amp;U62</f>
         <v>"TTCT","TATG","TTAG","TTTT"</v>
@@ -2358,13 +2351,16 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="P59:P62"/>
-    <mergeCell ref="P3:P6"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="P24:P27"/>
-    <mergeCell ref="P31:P34"/>
-    <mergeCell ref="P38:P41"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="Q16:T16"/>
+    <mergeCell ref="Q23:T23"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="J9:M9"/>
     <mergeCell ref="Q30:T30"/>
     <mergeCell ref="Q44:T44"/>
     <mergeCell ref="Q51:T51"/>
@@ -2378,16 +2374,13 @@
     <mergeCell ref="Q37:T37"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C23:F23"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="Q9:T9"/>
-    <mergeCell ref="Q16:T16"/>
-    <mergeCell ref="Q23:T23"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="I3:I6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="P59:P62"/>
+    <mergeCell ref="P3:P6"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="P17:P20"/>
+    <mergeCell ref="P24:P27"/>
+    <mergeCell ref="P31:P34"/>
+    <mergeCell ref="P38:P41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2395,73 +2388,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="Z34" sqref="Z34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16:P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="6"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" customWidth="1"/>
-    <col min="14" max="14" width="16.453125" customWidth="1"/>
-    <col min="15" max="15" width="8.81640625" style="6"/>
-    <col min="16" max="17" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="6"/>
+    <col min="16" max="17" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="1.90625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:26" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="55"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="43"/>
       <c r="O2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="43" t="s">
+      <c r="P2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="45"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="51"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="46">
         <v>16</v>
       </c>
@@ -2537,7 +2530,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="47"/>
       <c r="C4" s="21" t="s">
         <v>0</v>
@@ -2609,7 +2602,7 @@
         <v>"AGTCAGTCCC"</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
       <c r="C5" s="21" t="s">
         <v>0</v>
@@ -2681,7 +2674,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="47"/>
       <c r="C6" s="21" t="s">
         <v>0</v>
@@ -2753,7 +2746,7 @@
         <v>"AGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="47"/>
       <c r="C7" s="23" t="s">
         <v>0</v>
@@ -2825,7 +2818,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="47"/>
       <c r="C8" s="23" t="s">
         <v>0</v>
@@ -2897,7 +2890,7 @@
         <v>"AGTCAGTCCC"</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
       <c r="C9" s="23" t="s">
         <v>0</v>
@@ -2918,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>3</v>
@@ -2931,7 +2924,7 @@
       </c>
       <c r="M9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>"ATCGATCGGG"</v>
+        <v>"ATCGATAGGG"</v>
       </c>
       <c r="O9" s="47"/>
       <c r="P9" s="32" t="s">
@@ -2969,7 +2962,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
       <c r="C10" s="23" t="s">
         <v>1</v>
@@ -3041,7 +3034,7 @@
         <v>"AGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
       <c r="C11" s="23" t="s">
         <v>2</v>
@@ -3113,7 +3106,7 @@
         <v>"CGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="48"/>
       <c r="C12" s="24" t="s">
         <v>3</v>
@@ -3186,9 +3179,9 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="57" t="str">
+      <c r="A13" s="45" t="str">
         <f>M3&amp;","&amp;M4&amp;","&amp;M5&amp;","&amp;M6&amp;","&amp;M7&amp;","&amp;M8&amp;","&amp;M9&amp;","&amp;M10&amp;","&amp;M11&amp;","&amp;M12</f>
-        <v>"ATCGATCGGG","AGTCAGTCCC","ATCGATCGGG","AGTCCGTCCC","ATCGATCGGG","AGTCAGTCCC","ATCGATCGGG","TGTCCGTCCC","CGTCCGTCCC","GGTCCGTCCC"</v>
+        <v>"ATCGATCGGG","AGTCAGTCCC","ATCGATCGGG","AGTCCGTCCC","ATCGATCGGG","AGTCAGTCCC","ATCGATAGGG","TGTCCGTCCC","CGTCCGTCCC","GGTCCGTCCC"</v>
       </c>
       <c r="B13" s="10"/>
       <c r="D13" s="7"/>
@@ -3201,7 +3194,7 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="57" t="str">
+      <c r="N13" s="45" t="str">
         <f>Z3&amp;","&amp;Z4&amp;","&amp;Z5&amp;","&amp;Z6&amp;","&amp;Z7&amp;","&amp;Z8&amp;","&amp;Z9&amp;","&amp;Z10&amp;","&amp;Z11&amp;","&amp;Z12</f>
         <v>"ATCGATCGGG","AGTCAGTCCC","ATCGATCGGG","AGTCCGTCCC","ATCGATCGGG","AGTCAGTCCC","ATCGATCGGG","AGTCCGTCCC","CGTCCGTCCC","GGTCCGTCCC"</v>
       </c>
@@ -3216,43 +3209,43 @@
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
-      <c r="Z13" s="56"/>
-    </row>
-    <row r="14" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Z13" s="44"/>
+    </row>
+    <row r="14" spans="1:26" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:26" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="55"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="43"/>
       <c r="O15" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="43" t="s">
+      <c r="P15" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="45"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="50"/>
+      <c r="X15" s="50"/>
+      <c r="Y15" s="51"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="46">
         <v>17</v>
       </c>
@@ -3328,7 +3321,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B17" s="47"/>
       <c r="C17" s="1" t="s">
         <v>3</v>
@@ -3400,7 +3393,7 @@
         <v>"AGTCAGTCCC"</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B18" s="47"/>
       <c r="C18" s="1" t="s">
         <v>2</v>
@@ -3472,7 +3465,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B19" s="47"/>
       <c r="C19" s="1" t="s">
         <v>2</v>
@@ -3544,7 +3537,7 @@
         <v>"AGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B20" s="47"/>
       <c r="C20" s="3" t="s">
         <v>0</v>
@@ -3616,7 +3609,7 @@
         <v>"AAAAATCGGG"</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B21" s="47"/>
       <c r="C21" s="3" t="s">
         <v>0</v>
@@ -3688,7 +3681,7 @@
         <v>"AGTCAGTCCC"</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B22" s="47"/>
       <c r="C22" s="3" t="s">
         <v>0</v>
@@ -3760,7 +3753,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B23" s="47"/>
       <c r="C23" s="3" t="s">
         <v>1</v>
@@ -3832,7 +3825,7 @@
         <v>"AGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B24" s="47"/>
       <c r="C24" s="3" t="s">
         <v>2</v>
@@ -3904,7 +3897,7 @@
         <v>"CGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="48"/>
       <c r="C25" s="17" t="s">
         <v>3</v>
@@ -3977,7 +3970,7 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="56" t="str">
+      <c r="A26" s="44" t="str">
         <f>M16&amp;","&amp;M17&amp;","&amp;M18&amp;","&amp;M19&amp;","&amp;M20&amp;","&amp;M21&amp;","&amp;M22&amp;","&amp;M23&amp;","&amp;M24&amp;","&amp;M25</f>
         <v>"ATCGATCGGG","GATCAGTCCC","CTAGATCGGG","CGTACGTCCC","ATCGATCGGG","AGTCAATCCC","ATCGATAGGG","TGTCCGTCCC","CGTCCGTCCC","GGTCCGTCCC"</v>
       </c>
@@ -3993,7 +3986,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="56" t="str">
+      <c r="N26" s="44" t="str">
         <f>Z16&amp;","&amp;Z17&amp;","&amp;Z18&amp;","&amp;Z19&amp;","&amp;Z20&amp;","&amp;Z21&amp;","&amp;Z22&amp;","&amp;Z23&amp;","&amp;Z24&amp;","&amp;Z25</f>
         <v>"ATCGATCGGG","AGTCAGTCCC","ATCGATCGGG","AGTCCGTCCC","AAAAATCGGG","AGTCAGTCCC","ATCGATCGGG","AGTCCGTCCC","CGTCCGTCCC","GGTCCGTCCC"</v>
       </c>
@@ -4009,41 +4002,41 @@
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
     </row>
-    <row r="27" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:26" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:26" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="55"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="43"/>
       <c r="O28" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="P28" s="43" t="s">
+      <c r="P28" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="Q28" s="44"/>
-      <c r="R28" s="44"/>
-      <c r="S28" s="44"/>
-      <c r="T28" s="44"/>
-      <c r="U28" s="44"/>
-      <c r="V28" s="44"/>
-      <c r="W28" s="44"/>
-      <c r="X28" s="44"/>
-      <c r="Y28" s="45"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="51"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B29" s="46">
         <v>18</v>
       </c>
@@ -4119,7 +4112,7 @@
         <v>"ATGCGTCGGG"</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B30" s="47"/>
       <c r="C30" s="3" t="s">
         <v>3</v>
@@ -4191,7 +4184,7 @@
         <v>"TAACGGTCCC"</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B31" s="47"/>
       <c r="C31" s="3" t="s">
         <v>2</v>
@@ -4263,7 +4256,7 @@
         <v>"GTAGGTCGGG"</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B32" s="47"/>
       <c r="C32" s="3" t="s">
         <v>2</v>
@@ -4335,7 +4328,7 @@
         <v>"TGCAGGTCCC"</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B33" s="47"/>
       <c r="C33" s="3" t="s">
         <v>0</v>
@@ -4407,7 +4400,7 @@
         <v>"CCCCATCGGG"</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B34" s="47"/>
       <c r="C34" s="3" t="s">
         <v>0</v>
@@ -4479,7 +4472,7 @@
         <v>"AGTCAGTCCC"</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B35" s="47"/>
       <c r="C35" s="3" t="s">
         <v>0</v>
@@ -4551,7 +4544,7 @@
         <v>"ATCGATCGGG"</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B36" s="47"/>
       <c r="C36" s="3" t="s">
         <v>1</v>
@@ -4623,7 +4616,7 @@
         <v>"TGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B37" s="47"/>
       <c r="C37" s="3" t="s">
         <v>2</v>
@@ -4695,7 +4688,7 @@
         <v>"CGTCCGTCCC"</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="48"/>
       <c r="C38" s="17" t="s">
         <v>3</v>
@@ -4768,17 +4761,22 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="56" t="str">
+      <c r="A39" s="44" t="str">
         <f>M29&amp;","&amp;M30&amp;","&amp;M31&amp;","&amp;M32&amp;","&amp;M33&amp;","&amp;M34&amp;","&amp;M35&amp;","&amp;M36&amp;","&amp;M37&amp;","&amp;M38</f>
         <v>"CTCGATCGGA","GTTCAGTCAC","CTGGATCAGG","CGTCCGACCC","ATCGAACGGG","AGTCAATCCC","ATCAATAGGG","TGTCCGTCCC","CGTCCGTCCC","GGTCCGTCCC"</v>
       </c>
-      <c r="N39" s="56" t="str">
+      <c r="N39" s="44" t="str">
         <f>Z29&amp;","&amp;Z30&amp;","&amp;Z31&amp;","&amp;Z32&amp;","&amp;Z33&amp;","&amp;Z34&amp;","&amp;Z35&amp;","&amp;Z36&amp;","&amp;Z37&amp;","&amp;Z38</f>
         <v>"ATGCGTCGGG","TAACGGTCCC","GTAGGTCGGG","TGCAGGTCCC","CCCCATCGGG","AGTCAGTCCC","ATCGATCGGG","TGTCCGTCCC","CGTCCGTCCC","GGTCCGTCCC"</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="P2:Y2"/>
+    <mergeCell ref="O3:O12"/>
+    <mergeCell ref="B16:B25"/>
     <mergeCell ref="B29:B38"/>
     <mergeCell ref="O29:O38"/>
     <mergeCell ref="O16:O25"/>
@@ -4786,42 +4784,37 @@
     <mergeCell ref="P15:Y15"/>
     <mergeCell ref="P28:Y28"/>
     <mergeCell ref="C28:L28"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="P2:Y2"/>
-    <mergeCell ref="O3:O12"/>
-    <mergeCell ref="B16:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1796875" customWidth="1"/>
-    <col min="4" max="4" width="6.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
       <c r="H3" s="41" t="s">
         <v>4</v>
       </c>
@@ -4833,7 +4826,7 @@
       <c r="L3" s="53"/>
       <c r="M3" s="54"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="46">
         <v>22</v>
       </c>
@@ -4850,7 +4843,7 @@
         <f>CONCATENATE(CHAR(34),C4,D4,E4,CHAR(34))</f>
         <v>"ATC"</v>
       </c>
-      <c r="H4" s="49">
+      <c r="H4" s="55">
         <v>25</v>
       </c>
       <c r="I4" s="36" t="s">
@@ -4873,7 +4866,7 @@
         <v>"ATCTT"</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
       <c r="C5" s="34" t="s">
         <v>0</v>
@@ -4888,7 +4881,7 @@
         <f t="shared" ref="F5:F7" si="0">CONCATENATE(CHAR(34),C5,D5,E5,CHAR(34))</f>
         <v>"AGT"</v>
       </c>
-      <c r="H5" s="50"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="5" t="s">
         <v>0</v>
       </c>
@@ -4909,7 +4902,7 @@
         <v>"AGTCC"</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="47"/>
       <c r="C6" s="34" t="s">
         <v>0</v>
@@ -4924,7 +4917,7 @@
         <f t="shared" si="0"/>
         <v>"ATC"</v>
       </c>
-      <c r="H6" s="50"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="5" t="s">
         <v>0</v>
       </c>
@@ -4945,7 +4938,7 @@
         <v>"ATCAA"</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="48"/>
       <c r="C7" s="35" t="s">
         <v>0</v>
@@ -4960,7 +4953,7 @@
         <f t="shared" si="0"/>
         <v>"AGT"</v>
       </c>
-      <c r="H7" s="51"/>
+      <c r="H7" s="57"/>
       <c r="I7" s="39" t="s">
         <v>0</v>
       </c>
@@ -4981,7 +4974,7 @@
         <v>"AGTAA"</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C8" t="str">
         <f>F4&amp;","&amp;F5&amp;","&amp;F6&amp;","&amp;F7</f>
         <v>"ATC","AGT","ATC","AGT"</v>
@@ -4991,18 +4984,18 @@
         <v>"ATCTT","AGTCC","ATCAA","AGTAA"</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="46">
         <v>23</v>
       </c>
@@ -5020,7 +5013,7 @@
         <v>"ATC"</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
       <c r="C12" s="34" t="s">
         <v>0</v>
@@ -5036,7 +5029,7 @@
         <v>"AGT"</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="48"/>
       <c r="C13" s="34" t="s">
         <v>0</v>
@@ -5052,25 +5045,25 @@
         <v>"ATC"</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C14" t="str">
         <f>F11&amp;","&amp;F12&amp;","&amp;F13</f>
         <v>"ATC","AGT","ATC"</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:14" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="51"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="46">
         <v>24</v>
       </c>
@@ -5091,7 +5084,7 @@
         <v>"BTCG"</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="47"/>
       <c r="C18" s="12" t="s">
         <v>0</v>
@@ -5110,7 +5103,7 @@
         <v>"AGTC"</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="47"/>
       <c r="C19" s="12" t="s">
         <v>0</v>
@@ -5129,7 +5122,7 @@
         <v>"ATCG"</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="48"/>
       <c r="C20" s="42" t="s">
         <v>0</v>
@@ -5148,7 +5141,7 @@
         <v>"AGTC"</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C21" t="str">
         <f>G17&amp;","&amp;G18&amp;","&amp;G19&amp;","&amp;G20</f>
         <v>"BTCG","AGTC","ATCG","AGTC"</v>

</xml_diff>